<commit_message>
delete and modify docs #5
</commit_message>
<xml_diff>
--- a/doc/parameter/parameter.xlsx
+++ b/doc/parameter/parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiros\Desktop\GitLab\homelab\doc\parameter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiros\Desktop\GitLab\homelabo\doc\parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3465ED-DD89-4B83-AA1C-53ADCEC6A991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5674BE0-83D0-4573-B100-90941033D17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{11DF6A9B-95F3-483E-979F-31E2CBE1FAAD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{11DF6A9B-95F3-483E-979F-31E2CBE1FAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="IP_address" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
   <si>
     <t>installed_host_type</t>
     <phoneticPr fontId="1"/>
@@ -399,22 +399,52 @@
     <t>192.168.10.XX</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>192.168.10.70</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev-test001v</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>dev-docker001v</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>192.168.10.70</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>192.168.10.71</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev-test001v</t>
+  </si>
+  <si>
+    <t>dev-flog001v</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev-flog002v</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>192.168.10.32</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>192.168.10.33</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>192.168.10.34</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>flog-vip</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>192.168.10.35</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev-repo001v</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -422,7 +452,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,7 +772,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -837,6 +867,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -857,9 +893,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -897,7 +933,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1003,7 +1039,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1145,7 +1181,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1153,19 +1189,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD913314-F4D5-4A01-89E4-FFBB52A4AD78}">
-  <dimension ref="B1:I34"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="2" max="4" width="16.9375" customWidth="1"/>
     <col min="5" max="6" width="13.8125" customWidth="1"/>
     <col min="7" max="8" width="11.4375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.75"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:9" ht="18" thickBot="1"/>
+    <row r="2" spans="2:9">
       <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
@@ -1180,7 +1218,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="3" spans="2:9">
       <c r="B3" s="13" t="s">
         <v>38</v>
       </c>
@@ -1203,7 +1241,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="4" spans="2:9">
       <c r="B4" s="21" t="s">
         <v>75</v>
       </c>
@@ -1218,7 +1256,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="5" spans="2:9">
       <c r="B5" s="21" t="s">
         <v>86</v>
       </c>
@@ -1233,7 +1271,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="6" spans="2:9">
       <c r="B6" s="21" t="s">
         <v>76</v>
       </c>
@@ -1244,7 +1282,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="7" spans="2:9">
       <c r="B7" s="15" t="s">
         <v>1</v>
       </c>
@@ -1263,7 +1301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="8" spans="2:9">
       <c r="B8" s="15" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="9" spans="2:9">
       <c r="B9" s="15"/>
       <c r="C9" s="5" t="s">
         <v>3</v>
@@ -1301,7 +1339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="10" spans="2:9">
       <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -1320,7 +1358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="11" spans="2:9">
       <c r="B11" s="15"/>
       <c r="C11" s="5" t="s">
         <v>91</v>
@@ -1339,7 +1377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="12" spans="2:9">
       <c r="B12" s="15"/>
       <c r="C12" s="5" t="s">
         <v>5</v>
@@ -1361,7 +1399,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="13" spans="2:9">
       <c r="B13" s="15"/>
       <c r="C13" s="5" t="s">
         <v>6</v>
@@ -1383,7 +1421,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="14" spans="2:9">
       <c r="B14" s="26"/>
       <c r="C14" s="27" t="s">
         <v>65</v>
@@ -1402,7 +1440,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="15" spans="2:9">
       <c r="B15" s="15"/>
       <c r="C15" s="5" t="s">
         <v>88</v>
@@ -1424,7 +1462,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.7">
+    <row r="16" spans="2:9">
       <c r="B16" s="15"/>
       <c r="C16" s="5" t="s">
         <v>7</v>
@@ -1446,7 +1484,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="17" spans="2:8">
       <c r="B17" s="26"/>
       <c r="C17" s="27" t="s">
         <v>66</v>
@@ -1465,7 +1503,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="18" spans="2:8">
       <c r="B18" s="15"/>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -1480,7 +1518,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="19" spans="2:8">
       <c r="B19" s="15"/>
       <c r="C19" s="5" t="s">
         <v>9</v>
@@ -1495,7 +1533,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="20" spans="2:8">
       <c r="B20" s="15"/>
       <c r="C20" s="5" t="s">
         <v>10</v>
@@ -1510,7 +1548,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="21" spans="2:8">
       <c r="B21" s="15"/>
       <c r="C21" s="5" t="s">
         <v>11</v>
@@ -1525,7 +1563,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="16"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="22" spans="2:8">
       <c r="B22" s="15"/>
       <c r="C22" s="5" t="s">
         <v>12</v>
@@ -1540,7 +1578,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="23" spans="2:8">
       <c r="B23" s="15"/>
       <c r="C23" s="5" t="s">
         <v>80</v>
@@ -1555,7 +1593,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="24" spans="2:8">
       <c r="B24" s="15"/>
       <c r="C24" s="5" t="s">
         <v>81</v>
@@ -1570,7 +1608,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="25" spans="2:8">
       <c r="B25" s="26"/>
       <c r="C25" s="27" t="s">
         <v>89</v>
@@ -1589,7 +1627,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="26" spans="2:8">
       <c r="B26" s="15"/>
       <c r="C26" s="5" t="s">
         <v>14</v>
@@ -1608,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="27" spans="2:8">
       <c r="B27" s="15"/>
       <c r="C27" s="5" t="s">
         <v>15</v>
@@ -1627,7 +1665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="28" spans="2:8">
       <c r="B28" s="15"/>
       <c r="C28" s="5" t="s">
         <v>16</v>
@@ -1646,7 +1684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="29" spans="2:8">
       <c r="B29" s="15"/>
       <c r="C29" s="5" t="s">
         <v>17</v>
@@ -1665,7 +1703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="30" spans="2:8">
       <c r="B30" s="15"/>
       <c r="C30" s="5" t="s">
         <v>18</v>
@@ -1684,7 +1722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="31" spans="2:8">
       <c r="B31" s="15"/>
       <c r="C31" s="5" t="s">
         <v>87</v>
@@ -1699,7 +1737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="32" spans="2:8">
       <c r="B32" s="29"/>
       <c r="C32" s="30" t="s">
         <v>13</v>
@@ -1718,17 +1756,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="33" spans="2:8">
       <c r="B33" s="29"/>
       <c r="C33" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G33" s="30">
         <v>4</v>
@@ -1737,24 +1775,127 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B34" s="17"/>
-      <c r="C34" s="18" t="s">
+    <row r="34" spans="2:8">
+      <c r="B34" s="29"/>
+      <c r="C34" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="18">
-        <v>4</v>
-      </c>
-      <c r="H34" s="19">
-        <v>4</v>
-      </c>
+      <c r="G34" s="30">
+        <v>4</v>
+      </c>
+      <c r="H34" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="33"/>
+      <c r="C35" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="29"/>
+      <c r="C36" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="30">
+        <v>4</v>
+      </c>
+      <c r="H36" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="29"/>
+      <c r="C37" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="30">
+        <v>4</v>
+      </c>
+      <c r="H37" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="29"/>
+      <c r="C38" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="30">
+        <v>2</v>
+      </c>
+      <c r="H38" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="31"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="31"/>
+    </row>
+    <row r="41" spans="2:8" ht="18" thickBot="1">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1768,12 +1909,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="2" max="3" width="22.4375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:3">
       <c r="B2" s="6" t="s">
         <v>59</v>
       </c>
@@ -1781,81 +1922,81 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="3" spans="2:3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="4" spans="2:3">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="5" spans="2:3">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="6" spans="2:3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="7" spans="2:3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="8" spans="2:3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="9" spans="2:3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="10" spans="2:3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="11" spans="2:3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="12" spans="2:3">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="13" spans="2:3">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="14" spans="2:3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="15" spans="2:3">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="16" spans="2:3">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="17" spans="2:3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="18" spans="2:3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="19" spans="2:3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="20" spans="2:3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.7">
+    <row r="21" spans="2:3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
@@ -1871,14 +2012,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.0625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.0625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:7">
       <c r="B2" s="2" t="s">
         <v>45</v>
       </c>
@@ -1892,7 +2033,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="3" spans="2:7">
       <c r="B3" t="s">
         <v>53</v>
       </c>
@@ -1906,7 +2047,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="4" spans="2:7">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -1914,22 +2055,22 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="7" spans="2:7">
       <c r="B7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="8" spans="2:7">
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="9" spans="2:7">
       <c r="C9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="10" spans="2:7">
       <c r="D10" s="3" t="s">
         <v>45</v>
       </c>
@@ -1943,23 +2084,23 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="11" spans="2:7">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="12" spans="2:7">
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="13" spans="2:7">
       <c r="C13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.7">
+    <row r="14" spans="2:7">
       <c r="D14" s="3" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
commit_rules.txt   - add file
troubleshooting_guide.txt
  - move directory

README.md
  - add detail and delete unneccecary line

00_playbook_command.txt
  - add ansible-playbook command for test one role and update material on Ansible server
  - delete ansible-playbook command for repo server

00_instruction_create_minikube.txt
  - modify install method

04_instruction_setup_nfsclient.txt
  - modify version infomation

05_instruction_create_ansible_server.txt
  - comment out
  - add description and delete line

09_instruction_create_zabbix_server.txt
  - delete lines

operation_kubectl_command.txt
  - add file

parameter.xlsx
  - modify content
</commit_message>
<xml_diff>
--- a/doc/parameter/parameter.xlsx
+++ b/doc/parameter/parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiros\Desktop\GitLab\homelabo\doc\parameter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiros\Desktop\GitLab\homelab\doc\parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5674BE0-83D0-4573-B100-90941033D17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8B8567-CC4E-4CF2-BD9C-82E308641B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{11DF6A9B-95F3-483E-979F-31E2CBE1FAAD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{11DF6A9B-95F3-483E-979F-31E2CBE1FAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="IP_address" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
   <si>
     <t>installed_host_type</t>
     <phoneticPr fontId="1"/>
@@ -437,14 +437,6 @@
   </si>
   <si>
     <t>flog-vip</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>192.168.10.35</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev-repo001v</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1191,9 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD913314-F4D5-4A01-89E4-FFBB52A4AD78}">
   <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
@@ -1853,22 +1843,12 @@
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="29"/>
-      <c r="C38" s="30" t="s">
-        <v>111</v>
-      </c>
+      <c r="C38" s="30"/>
       <c r="D38" s="30"/>
-      <c r="E38" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="G38" s="30">
-        <v>2</v>
-      </c>
-      <c r="H38" s="31">
-        <v>2</v>
-      </c>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="31"/>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="29"/>

</xml_diff>